<commit_message>
Appium Sample on Nearbuy app
</commit_message>
<xml_diff>
--- a/test_data/NearBuy_Test_Cases_V1.xlsx
+++ b/test_data/NearBuy_Test_Cases_V1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivaprasad.a\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mobile\robotframework-appium-sample2\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF271AA-A8A8-4A30-B2AF-914A68CADB00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C900D82D-131F-4C1C-BBB0-CC36A436A1C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8789ECDF-C16A-4FF0-A906-20FEE485B5B3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>S.No</t>
   </si>
@@ -57,27 +57,9 @@
     <t>Validate install NearBuy application</t>
   </si>
   <si>
-    <t>Validate available fields in home page</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
-    <t>Validate menu fields</t>
-  </si>
-  <si>
-    <t>Validate quick icons in home page</t>
-  </si>
-  <si>
-    <t>Validate search in application</t>
-  </si>
-  <si>
-    <t>Validate scroll in home &amp; search results</t>
-  </si>
-  <si>
-    <t>Validate more icon on scroll</t>
-  </si>
-  <si>
     <t>Validate app running in back groud</t>
   </si>
   <si>
@@ -88,6 +70,66 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Validate Available Standard Icons In Home Screen</t>
+  </si>
+  <si>
+    <t>Validate Available Quick Search Icons In Home Screen</t>
+  </si>
+  <si>
+    <t>Validate Search Functionality In Home Screen</t>
+  </si>
+  <si>
+    <t>Validate Notifications In Home Screen</t>
+  </si>
+  <si>
+    <t>Validate Available Menu Fields In Home Screen</t>
+  </si>
+  <si>
+    <t>Validate Search Functionality In Search Screen</t>
+  </si>
+  <si>
+    <t>Validate Back Button Functionality In Search Screen</t>
+  </si>
+  <si>
+    <t>Validate View Details Of Search Record</t>
+  </si>
+  <si>
+    <t>Validate Add To Favourites Of Search Record</t>
+  </si>
+  <si>
+    <t>Validate Sort Search Record Using 'Near Me' Option</t>
+  </si>
+  <si>
+    <t>Validate Refresh By Dragging Down In Search Result Screen</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Automated</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Can be automated using desired capability fullReset</t>
+  </si>
+  <si>
+    <t>Validate Scroll In Search Screen</t>
+  </si>
+  <si>
+    <t>Validate Scroll Down In Home Screen</t>
+  </si>
+  <si>
+    <t>Validate Scroll Up In Home Screen</t>
+  </si>
+  <si>
+    <t>Validate Nearbuy Blog Link</t>
   </si>
 </sst>
 </file>
@@ -137,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,6 +189,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,22 +510,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC7C1CD-44B1-46C2-8BB4-3C17BD128897}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.109375" customWidth="1"/>
-    <col min="2" max="2" width="38.44140625" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.21875" style="3" customWidth="1"/>
     <col min="4" max="4" width="15.21875" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,8 +542,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -502,10 +554,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -513,96 +571,264 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Include search test cases
</commit_message>
<xml_diff>
--- a/test_data/NearBuy_Test_Cases_V1.xlsx
+++ b/test_data/NearBuy_Test_Cases_V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mobile\robotframework-appium-sample2\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C900D82D-131F-4C1C-BBB0-CC36A436A1C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33DCC3E-46AE-4165-9523-032F1F447E85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8789ECDF-C16A-4FF0-A906-20FEE485B5B3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="34">
   <si>
     <t>S.No</t>
   </si>
@@ -87,21 +87,12 @@
     <t>Validate Available Menu Fields In Home Screen</t>
   </si>
   <si>
-    <t>Validate Search Functionality In Search Screen</t>
-  </si>
-  <si>
-    <t>Validate Back Button Functionality In Search Screen</t>
-  </si>
-  <si>
     <t>Validate View Details Of Search Record</t>
   </si>
   <si>
     <t>Validate Add To Favourites Of Search Record</t>
   </si>
   <si>
-    <t>Validate Sort Search Record Using 'Near Me' Option</t>
-  </si>
-  <si>
     <t>Validate Refresh By Dragging Down In Search Result Screen</t>
   </si>
   <si>
@@ -120,9 +111,6 @@
     <t>Can be automated using desired capability fullReset</t>
   </si>
   <si>
-    <t>Validate Scroll In Search Screen</t>
-  </si>
-  <si>
     <t>Validate Scroll Down In Home Screen</t>
   </si>
   <si>
@@ -130,6 +118,24 @@
   </si>
   <si>
     <t>Validate Nearbuy Blog Link</t>
+  </si>
+  <si>
+    <t>Validate app when no internet connection</t>
+  </si>
+  <si>
+    <t>Validate Sort Search Record Using 'Rating' Option</t>
+  </si>
+  <si>
+    <t>Validate Search &amp; Back Functionality In Search Screen</t>
+  </si>
+  <si>
+    <t>Validate Scroll Up In Search Results</t>
+  </si>
+  <si>
+    <t>Validate Scroll Down In Search Results</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -510,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC7C1CD-44B1-46C2-8BB4-3C17BD128897}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -557,10 +563,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -574,7 +580,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -589,10 +595,10 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" s="5"/>
     </row>
@@ -607,10 +613,10 @@
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="5"/>
     </row>
@@ -619,16 +625,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -637,16 +643,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -661,10 +667,10 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F8" s="5"/>
     </row>
@@ -679,10 +685,10 @@
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -697,10 +703,10 @@
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F10" s="5"/>
     </row>
@@ -709,16 +715,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -727,10 +733,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -739,10 +751,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F13" s="5"/>
     </row>
@@ -751,10 +769,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F14" s="5"/>
     </row>
@@ -763,10 +787,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F15" s="5"/>
     </row>
@@ -775,10 +805,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F16" s="5"/>
     </row>
@@ -787,10 +823,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -799,10 +841,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F18" s="5"/>
     </row>
@@ -816,6 +864,12 @@
       <c r="C19" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -828,7 +882,30 @@
       <c r="C20" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>